<commit_message>
UofR data cleaning pt2
</commit_message>
<xml_diff>
--- a/04_notes/Data Cleaning Notes.xlsx
+++ b/04_notes/Data Cleaning Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessi\OneDrive\Desktop\Jess\LDP Internship\LDP-Internship\04_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371A9367-499F-495C-AE6D-00D214422377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB2734B-1C5E-4F96-BF8E-285152987D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{44EE4F3D-387E-4BE5-B9A2-F7B5EB58756F}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
-  <si>
-    <t>Raw Data Files</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Sheet/Tab</t>
   </si>
@@ -99,6 +96,39 @@
   </si>
   <si>
     <t xml:space="preserve">Tidy Data File </t>
+  </si>
+  <si>
+    <t>All_Data_PPR_2006_to_2024 MASTER FILE</t>
+  </si>
+  <si>
+    <t>Absorbance</t>
+  </si>
+  <si>
+    <t>Field Stats</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Data PPR 2006 COMPLETE April 2009</t>
+  </si>
+  <si>
+    <t>01_Datacleanup</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>PPR_merged_2006-2024</t>
+  </si>
+  <si>
+    <t>SDWS_merged_2014-2022</t>
+  </si>
+  <si>
+    <t>Raw Data Files (or Tidy Data Files)</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
@@ -122,12 +152,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -160,21 +208,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,223 +583,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C599B0-8B6A-4908-988B-60DB6FD458CC}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="B2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="C14:C21"/>
-    <mergeCell ref="D14:D21"/>
+  <mergeCells count="14">
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="D2:D9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="D10:D13"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="C14:C21"/>
+    <mergeCell ref="D14:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final data cleaning, converting to long format
</commit_message>
<xml_diff>
--- a/04_notes/Data Cleaning Notes.xlsx
+++ b/04_notes/Data Cleaning Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessi\OneDrive\Desktop\Jess\LDP Internship\LDP-Internship\04_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB2734B-1C5E-4F96-BF8E-285152987D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D56239D-781A-436D-A7DD-670AD8A5DF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{44EE4F3D-387E-4BE5-B9A2-F7B5EB58756F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>Sheet/Tab</t>
   </si>
@@ -129,6 +129,33 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>Baulch_2015-2022</t>
+  </si>
+  <si>
+    <t>SDWS_Baulch_merged_2014-2022</t>
+  </si>
+  <si>
+    <t>Robbins_2023</t>
+  </si>
+  <si>
+    <t>TICTOC_2021-2023</t>
+  </si>
+  <si>
+    <t>THG_data_2021</t>
+  </si>
+  <si>
+    <t>SDWS 2015-2022 Baulch</t>
+  </si>
+  <si>
+    <t>L.Robbins Lab Data 2021-2023 - SW Sed PW chem data.xlsx - Sediment bulk TM [clean]</t>
+  </si>
+  <si>
+    <t>TICTOC Results May 30, 2023</t>
+  </si>
+  <si>
+    <t>DMA-80 THG Data_Cleandata</t>
   </si>
 </sst>
 </file>
@@ -152,7 +179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,8 +204,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -204,17 +243,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -247,6 +296,35 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -255,6 +333,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -583,18 +667,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C599B0-8B6A-4908-988B-60DB6FD458CC}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -615,13 +699,13 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -629,69 +713,69 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="10"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="10"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="10"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="10"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="11"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -699,37 +783,37 @@
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="12"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="14"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -737,69 +821,69 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="16"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="16"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="16"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="17"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -807,67 +891,138 @@
       <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>14</v>
+      <c r="A27" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
+      <c r="D27" s="18"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
+      <c r="A28" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
+  <mergeCells count="17">
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="D2:D9"/>
@@ -879,6 +1034,8 @@
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="C14:C21"/>
     <mergeCell ref="D14:D21"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>